<commit_message>
format final result and delete duplicate ch_stress file
</commit_message>
<xml_diff>
--- a/results/tables/approaches/final_result.xlsx
+++ b/results/tables/approaches/final_result.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johannesallgaier/PycharmProjects/UsAs/results/tables/approaches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{68D0CF2F-6E20-2347-B4FD-3F14D3EC6137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A992577-DD25-C942-AA38-E23FD531EABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34440" yWindow="2020" windowWidth="38720" windowHeight="17440"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="final_result" sheetId="1" r:id="rId1"/>
@@ -20,27 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>average_rank_std_random</t>
-  </si>
-  <si>
-    <t xml:space="preserve">average_rank </t>
-  </si>
-  <si>
-    <t xml:space="preserve">average_rank_std </t>
-  </si>
-  <si>
-    <t xml:space="preserve">average_rank_random </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t xml:space="preserve">time_cut </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bl_user_based_last </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bl_user_based_all </t>
   </si>
   <si>
     <t xml:space="preserve">user_cut </t>
@@ -52,22 +34,36 @@
     <t xml:space="preserve">user_wise </t>
   </si>
   <si>
-    <t xml:space="preserve">bl_assessment_based_last </t>
+    <t>Users
+sorted by time</t>
   </si>
   <si>
-    <t xml:space="preserve">bl_assessment_based_all </t>
+    <t>Users
+split randomly</t>
   </si>
   <si>
-    <t>Users sorted by time</t>
+    <t>Average rank</t>
   </si>
   <si>
-    <t>Users split randomly</t>
+    <t>Std of average rank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BL user_based last </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BL user_based all </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BL assessment_based last </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BL assessment_based all </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -396,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -513,31 +509,11 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -550,12 +526,23 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -605,30 +592,32 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -983,180 +972,179 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="210" zoomScaleNormal="179" zoomScaleSheetLayoutView="315" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="23.83203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="5" width="20.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="4"/>
+    <row r="1" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
+    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="13">
+      <c r="B3" s="5">
         <v>2.29</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="6">
         <v>1.5</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1.5720000000000001</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.15702199999999999</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="13">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
         <v>3.57</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="6">
         <v>1.72</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>3.056</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.112</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="13">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
         <v>3.29</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="6">
         <v>1.7</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>3.46</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0.20957100000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="13">
+      <c r="A6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5">
         <v>3.86</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="6">
         <v>0.69</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>3.5139999999999998</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>0.35533599999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5">
         <v>3.57</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="6">
         <v>2.37</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>4.43</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>0.177088</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="13">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5">
         <v>4.33</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="6">
         <v>2.0699999999999998</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>5.1020000000000003</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>0.37541400000000003</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="5">
         <v>6.86</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="6">
         <v>0.69</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>6.8019999999999996</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>0.11600000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="5">
         <v>7.71</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="6">
         <v>0.49</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>7.6559999999999997</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>0.14554700000000001</v>
       </c>
     </row>
@@ -1169,6 +1157,16 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B10">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1178,7 +1176,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D10">
+  <conditionalFormatting sqref="C3:C10 E3:E10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1189,5 +1187,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="75" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change formats of tables according to editor
</commit_message>
<xml_diff>
--- a/results/tables/approaches/final_result.xlsx
+++ b/results/tables/approaches/final_result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johannesallgaier/PycharmProjects/UsAs/results/tables/approaches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A992577-DD25-C942-AA38-E23FD531EABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FEE89C-DC9B-A641-9A29-B3F4A06B760A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="final_result" sheetId="1" r:id="rId1"/>
@@ -602,12 +602,6 @@
     </xf>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -617,6 +611,12 @@
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -976,7 +976,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="210" zoomScaleNormal="179" zoomScaleSheetLayoutView="315" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.25"/>
@@ -988,27 +988,27 @@
   <sheetData>
     <row r="1" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1156,36 +1156,6 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:B10">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D10">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C10 E3:E10">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>